<commit_message>
Validaciones en la carga de lotes
</commit_message>
<xml_diff>
--- a/public/plantilla.xlsx
+++ b/public/plantilla.xlsx
@@ -13,15 +13,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>nombre</t>
   </si>
   <si>
     <t>descripcion</t>
-  </si>
-  <si>
-    <t>cantidad</t>
   </si>
   <si>
     <t>precio_venta</t>
@@ -97,16 +94,13 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -114,8 +108,8 @@
     <xf fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -632,86 +626,77 @@
   <cols>
     <col customWidth="1" min="1" max="1" style="2" width="22.421875"/>
     <col customWidth="1" min="2" max="2" style="2" width="35.28125"/>
-    <col customWidth="1" min="3" max="3" style="3" width="11.8515625"/>
-    <col customWidth="1" min="4" max="4" style="2" width="21.8515625"/>
-    <col customWidth="1" min="5" max="5" style="2" width="15.00390625"/>
-    <col customWidth="1" min="6" max="6" style="2" width="21.421875"/>
-    <col customWidth="1" min="7" max="7" style="1" width="19.28125"/>
-    <col customWidth="1" min="8" max="8" style="1" width="13.140625"/>
-    <col min="9" max="16384" style="1" width="9.140625"/>
+    <col customWidth="1" min="3" max="3" style="2" width="21.8515625"/>
+    <col customWidth="1" min="4" max="4" style="2" width="15.00390625"/>
+    <col customWidth="1" min="5" max="5" style="2" width="21.421875"/>
+    <col customWidth="1" min="6" max="6" style="1" width="19.28125"/>
+    <col customWidth="1" min="7" max="7" style="1" width="13.140625"/>
+    <col min="8" max="16384" style="1" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" ht="18">
-      <c r="A1" s="5" t="s">
+    <row r="1" s="3" customFormat="1" ht="18">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="6"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="6"/>
+      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="6"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="6"/>
+      <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="6"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Validaciones en la tabla
</commit_message>
<xml_diff>
--- a/public/plantilla.xlsx
+++ b/public/plantilla.xlsx
@@ -6,7 +6,7 @@
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="hoja1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <calcPr/>
 </workbook>
@@ -94,22 +94,12 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -618,85 +608,36 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" style="2" width="22.421875"/>
-    <col customWidth="1" min="2" max="2" style="2" width="35.28125"/>
-    <col customWidth="1" min="3" max="3" style="2" width="21.8515625"/>
-    <col customWidth="1" min="4" max="4" style="2" width="15.00390625"/>
-    <col customWidth="1" min="5" max="5" style="2" width="21.421875"/>
-    <col customWidth="1" min="6" max="6" style="1" width="19.28125"/>
-    <col customWidth="1" min="7" max="7" style="1" width="13.140625"/>
-    <col min="8" max="16384" style="1" width="9.140625"/>
+    <col customWidth="1" min="1" max="1" style="2" width="16.140625"/>
+    <col customWidth="1" min="2" max="2" style="2" width="47.140625"/>
+    <col customWidth="1" min="3" max="3" style="2" width="17.140625"/>
+    <col customWidth="1" min="4" max="4" style="2" width="20.28125"/>
+    <col customWidth="1" min="5" max="5" style="2" width="21.57421875"/>
+    <col min="6" max="16384" style="1" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" ht="18">
-      <c r="A1" s="4" t="s">
+    <row r="1" ht="18">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" ht="14.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" ht="14.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" ht="14.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" ht="14.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" ht="14.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>